<commit_message>
Cambios en el Documento
Es desarrollo la metodologia del documento.
</commit_message>
<xml_diff>
--- a/Proyecto de grado IIND/1. Datos/5. Estadisticas_Descriptivas.xlsx
+++ b/Proyecto de grado IIND/1. Datos/5. Estadisticas_Descriptivas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\windows\Documents\GitHub\Problem_Set_1\Proyecto-de-grado-IIND\Proyecto de grado IIND\1. Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477CDC83-F5D5-4B87-8EB0-A98215D6B4D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604068A2-A8F6-43B7-AE51-68A9B11CFB79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="3015" windowWidth="15375" windowHeight="7785" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -31,28 +31,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -869,11 +847,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F34DE168-3E16-4373-8DD2-B1DD3B33286F}">
-  <dimension ref="A1:Q110"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -882,7 +858,7 @@
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -895,42 +871,8 @@
       <c r="D1" t="s">
         <v>136</v>
       </c>
-      <c r="G1" t="str" cm="1">
-        <f t="array" ref="G1:Q1">TRANSPOSE(_xlfn.UNIQUE(A2:A110))</f>
-        <v xml:space="preserve">      o3</v>
-      </c>
-      <c r="H1" t="str">
-        <v xml:space="preserve">     no2</v>
-      </c>
-      <c r="I1" t="str">
-        <v xml:space="preserve">     pm25</v>
-      </c>
-      <c r="J1" t="str">
-        <v xml:space="preserve">      co</v>
-      </c>
-      <c r="K1" t="str">
-        <v xml:space="preserve">     so2</v>
-      </c>
-      <c r="L1" t="str">
-        <v xml:space="preserve">     pm10</v>
-      </c>
-      <c r="M1" t="str">
-        <v xml:space="preserve">      rh</v>
-      </c>
-      <c r="N1" t="str">
-        <v xml:space="preserve">     rain</v>
-      </c>
-      <c r="O1" t="str">
-        <v xml:space="preserve">   radsolar</v>
-      </c>
-      <c r="P1" t="str">
-        <v xml:space="preserve">      bc</v>
-      </c>
-      <c r="Q1" t="str">
-        <v xml:space="preserve">     co2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -944,12 +886,8 @@
         <f t="shared" ref="D2:D65" si="0">IFERROR(_xlfn.NUMBERVALUE(MID(B2,FIND(":",B2)+1,LEN(B2)*FIND(":",B2)),"."),"")</f>
         <v>11.015000000000001</v>
       </c>
-      <c r="F2" cm="1">
-        <f t="array" ref="F2:F14">+_xlfn.SEQUENCE(13,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -963,15 +901,8 @@
         <f t="shared" si="0"/>
         <v>9.9600000000000009</v>
       </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G14" si="1">+LARGE($D$2:$D$110,F3)</f>
-        <v>165.92599999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -985,15 +916,8 @@
         <f t="shared" si="0"/>
         <v>14.372999999999999</v>
       </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="1"/>
-        <v>160.024</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1007,15 +931,8 @@
         <f t="shared" si="0"/>
         <v>0.32650000000000001</v>
       </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="1"/>
-        <v>159.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1029,15 +946,8 @@
         <f t="shared" si="0"/>
         <v>1.4965999999999999</v>
       </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="1"/>
-        <v>153.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1051,15 +961,8 @@
         <f t="shared" si="0"/>
         <v>28.02</v>
       </c>
-      <c r="F7">
-        <v>6</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="1"/>
-        <v>150.03</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1073,15 +976,8 @@
         <f t="shared" si="0"/>
         <v>68.66</v>
       </c>
-      <c r="F8">
-        <v>7</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="1"/>
-        <v>145.63999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1095,15 +991,8 @@
         <f t="shared" si="0"/>
         <v>0.115343</v>
       </c>
-      <c r="F9">
-        <v>8</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="1"/>
-        <v>72.760000000000005</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1117,15 +1006,8 @@
         <f t="shared" si="0"/>
         <v>160.024</v>
       </c>
-      <c r="F10">
-        <v>9</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="1"/>
-        <v>70.86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1139,15 +1021,8 @@
         <f t="shared" si="0"/>
         <v>13.071</v>
       </c>
-      <c r="F11">
-        <v>10</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="1"/>
-        <v>69.7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1161,15 +1036,8 @@
         <f t="shared" si="0"/>
         <v>15.127000000000001</v>
       </c>
-      <c r="F12">
-        <v>11</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="1"/>
-        <v>68.66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1183,15 +1051,12 @@
         <f t="shared" si="0"/>
         <v>14.266999999999999</v>
       </c>
-      <c r="F13">
-        <v>12</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="1"/>
-        <v>68.45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G13" t="e">
+        <f t="shared" ref="G3:G14" si="1">+LARGE($D$2:$D$110,F13)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1205,15 +1070,12 @@
         <f t="shared" si="0"/>
         <v>0.73709999999999998</v>
       </c>
-      <c r="F14">
-        <v>13</v>
-      </c>
-      <c r="G14">
+      <c r="G14" t="e">
         <f t="shared" si="1"/>
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1228,7 +1090,7 @@
         <v>22.239000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -2664,7 +2526,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3AC713B-A20A-48AA-BDE5-14ACE492285B}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2883,7 +2747,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection sqref="A1:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3096,8 +2960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30EF78A9-90AA-461D-B3BA-DF90B674B1F6}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3177,13 +3041,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="D6">
-        <v>15.95</v>
+        <v>18.579000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3191,13 +3055,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="D7">
-        <v>15.127000000000001</v>
+        <v>15.95</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3205,13 +3069,13 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="D8">
-        <v>13.597</v>
+        <v>15.127000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3219,13 +3083,13 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s">
-        <v>123</v>
+        <v>63</v>
       </c>
       <c r="D9">
-        <v>13.195</v>
+        <v>13.597</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3233,13 +3097,13 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>125</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>123</v>
       </c>
       <c r="D10">
-        <v>12.31</v>
+        <v>13.195</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3247,13 +3111,13 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D11">
-        <v>12.085000000000001</v>
+        <v>12.31</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3261,13 +3125,13 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D12">
-        <v>10.375</v>
+        <v>12.085000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3275,13 +3139,13 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="D13">
-        <v>9.9600000000000009</v>
+        <v>10.375</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3289,13 +3153,13 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>18.579000000000001</v>
+        <v>9.9600000000000009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>